<commit_message>
Add apache poi to deal with the excel data of the order setting, now you can import the row data in the excel file to the database table though the poi tools made by myself a moment ago.
</commit_message>
<xml_diff>
--- a/health-backend/src/main/resources/file/orderSetting_template.xlsx
+++ b/health-backend/src/main/resources/file/orderSetting_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\health\health-backend\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D545A4-616D-4824-9793-68704404F906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02086D8B-DC75-4957-9480-EA0D3D7C66AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,13 +30,13 @@
     <t>序号</t>
   </si>
   <si>
-    <t>时间</t>
-  </si>
-  <si>
     <t>可预约人数</t>
   </si>
   <si>
     <t>已预约人数</t>
+  </si>
+  <si>
+    <t>日期</t>
   </si>
 </sst>
 </file>
@@ -72,8 +72,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,26 +359,32 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="11.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>